<commit_message>
collect Binance historical data
</commit_message>
<xml_diff>
--- a/backend/historical_data/binance_ticker.xlsx
+++ b/backend/historical_data/binance_ticker.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PalitoE\Downloads\palitoj_endthen\investment\apexlabs_material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PalitoE\Downloads\palitoj_endthen\investment\apexlabs\backend\historical_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{393E7D57-298A-4F6C-BDAD-B5A3227DE732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8C0421-106A-41C1-9366-A8C57FD9BFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D634B153-C235-4CC5-822F-8EA274D28C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$37</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="77">
   <si>
     <t>base</t>
   </si>
@@ -95,24 +98,12 @@
     <t>LTC</t>
   </si>
   <si>
-    <t>LEO</t>
-  </si>
-  <si>
-    <t>CRO</t>
-  </si>
-  <si>
-    <t>SHIB</t>
-  </si>
-  <si>
     <t>TON</t>
   </si>
   <si>
     <t>DOT</t>
   </si>
   <si>
-    <t>MNT</t>
-  </si>
-  <si>
     <t>XMR</t>
   </si>
   <si>
@@ -125,12 +116,6 @@
     <t>ENA</t>
   </si>
   <si>
-    <t>PEPE</t>
-  </si>
-  <si>
-    <t>OKB</t>
-  </si>
-  <si>
     <t>NEAR</t>
   </si>
   <si>
@@ -174,6 +159,117 @@
   </si>
   <si>
     <t>QNT</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Bitcoin</t>
+  </si>
+  <si>
+    <t>Ethereum</t>
+  </si>
+  <si>
+    <t>Ripple</t>
+  </si>
+  <si>
+    <t>Solana</t>
+  </si>
+  <si>
+    <t>Dogecoin</t>
+  </si>
+  <si>
+    <t>Tron</t>
+  </si>
+  <si>
+    <t>Cardano</t>
+  </si>
+  <si>
+    <t>Chailink</t>
+  </si>
+  <si>
+    <t>Hyperliquid</t>
+  </si>
+  <si>
+    <t>Sui</t>
+  </si>
+  <si>
+    <t>Stellar</t>
+  </si>
+  <si>
+    <t>Avalanche</t>
+  </si>
+  <si>
+    <t>Hedera</t>
+  </si>
+  <si>
+    <t>Litecoin</t>
+  </si>
+  <si>
+    <t>Toncoin</t>
+  </si>
+  <si>
+    <t>Polkadot</t>
+  </si>
+  <si>
+    <t>Monero</t>
+  </si>
+  <si>
+    <t>Uniswap</t>
+  </si>
+  <si>
+    <t>Aave</t>
+  </si>
+  <si>
+    <t>Ethena</t>
+  </si>
+  <si>
+    <t>Near Protocol</t>
+  </si>
+  <si>
+    <t>Aptos</t>
+  </si>
+  <si>
+    <t>Ondo</t>
+  </si>
+  <si>
+    <t>Bittensor</t>
+  </si>
+  <si>
+    <t>Worldcoin</t>
+  </si>
+  <si>
+    <t>Polygon (ex-Matic)</t>
+  </si>
+  <si>
+    <t>Internet Computer</t>
+  </si>
+  <si>
+    <t>Zcash</t>
+  </si>
+  <si>
+    <t>Arbitrum</t>
+  </si>
+  <si>
+    <t>VeChain</t>
+  </si>
+  <si>
+    <t>Cosmos</t>
+  </si>
+  <si>
+    <t>Algorand</t>
+  </si>
+  <si>
+    <t>Render</t>
+  </si>
+  <si>
+    <t>Filecoin</t>
+  </si>
+  <si>
+    <t>Quant</t>
   </si>
 </sst>
 </file>
@@ -209,8 +305,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,525 +642,679 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8D9E5B-7C36-4288-85B8-327E59D76B4F}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="str">
-        <f>A2&amp;B2</f>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="str">
+        <f>C2&amp;D2</f>
         <v>BTCUSDT</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C43" si="0">A3&amp;B3</f>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E37" si="0">C3&amp;D3</f>
         <v>ETHUSDT</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="str">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="str">
         <f t="shared" si="0"/>
         <v>XRPUSDT</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="str">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="str">
         <f t="shared" si="0"/>
         <v>BNBUSDT</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="str">
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>SOLUSDT</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="str">
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="str">
         <f t="shared" si="0"/>
         <v>DOGEUSDT</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="str">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="str">
         <f t="shared" si="0"/>
         <v>TRXUSDT</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="str">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="str">
         <f t="shared" si="0"/>
         <v>ADAUSDT</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="str">
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="str">
         <f t="shared" si="0"/>
         <v>LINKUSDT</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="str">
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>HYPEUSDT</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="str">
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="str">
         <f t="shared" si="0"/>
         <v>SUIUSDT</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="str">
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>XLMUSDT</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="str">
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="str">
         <f t="shared" si="0"/>
         <v>AVAXUSDT</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="str">
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="str">
         <f t="shared" si="0"/>
         <v>HBARUSDT</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="str">
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="str">
         <f t="shared" si="0"/>
         <v>LTCUSDT</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>LEOUSDT</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>TONUSDT</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>CROUSDT</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>DOTUSDT</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>SHIBUSDT</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>XMRUSDT</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>TONUSDT</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>UNIUSDT</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>DOTUSDT</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>AAVEUSDT</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>MNTUSDT</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>ENAUSDT</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>XMRUSDT</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>NEARUSDT</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v>UNIUSDT</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>APTUSDT</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>AAVEUSDT</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>ONDOUSDT</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>ENAUSDT</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>TAOUSDT</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v>PEPEUSDT</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>WLDUSDT</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v>OKBUSDT</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>POLUSDT</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v>NEARUSDT</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>ICPUSDT</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>APTUSDT</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>ZECUSDT</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" t="str">
-        <f t="shared" si="0"/>
-        <v>ONDOUSDT</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>ARBUSDT</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
         <v>34</v>
       </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v>TAOUSDT</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>VETUSDT</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
         <v>35</v>
       </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="str">
-        <f t="shared" si="0"/>
-        <v>WLDUSDT</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>ATOMUSDT</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" t="s">
         <v>36</v>
       </c>
-      <c r="B34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" t="str">
-        <f t="shared" si="0"/>
-        <v>POLUSDT</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>ALGOUSDT</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
         <v>37</v>
       </c>
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" t="str">
-        <f t="shared" si="0"/>
-        <v>ICPUSDT</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>RENDERUSDT</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
         <v>38</v>
       </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="str">
-        <f t="shared" si="0"/>
-        <v>ZECUSDT</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>FILUSDT</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
         <v>39</v>
       </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" t="str">
-        <f t="shared" si="0"/>
-        <v>ARBUSDT</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" t="str">
-        <f t="shared" si="0"/>
-        <v>VETUSDT</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" t="str">
-        <f t="shared" si="0"/>
-        <v>ATOMUSDT</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" t="str">
-        <f t="shared" si="0"/>
-        <v>ALGOUSDT</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" t="str">
-        <f t="shared" si="0"/>
-        <v>RENDERUSDT</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" t="str">
-        <f t="shared" si="0"/>
-        <v>FILUSDT</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" t="str">
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" t="str">
         <f t="shared" si="0"/>
         <v>QNTUSDT</v>
       </c>

</xml_diff>